<commit_message>
Add foreign key tests
- Includes fix to show original Lectern error when it doesn't need to be changed.
- Update Excel test files as original valid file wasn't valid anymore with the unique constraints
</commit_message>
<xml_diff>
--- a/tests/integration/test_files/invalid_code_list.xlsx
+++ b/tests/integration/test_files/invalid_code_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmartinez/repos/set-aside/pdcm-lectern-validator/tests/integration/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D18E6C-CD0E-1D4B-AB25-4B7AFAE3084D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FFEE8D-88ED-2D47-ACAF-38B559EB166A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17900" yWindow="3060" windowWidth="19300" windowHeight="11680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10420" yWindow="6180" windowWidth="29040" windowHeight="11680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="patient" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="123">
   <si>
     <t>patient_id</t>
   </si>
@@ -408,9 +408,6 @@
     <t>histo</t>
   </si>
   <si>
-    <t>CRC0s228PR</t>
-  </si>
-  <si>
     <t>NOD</t>
   </si>
   <si>
@@ -441,9 +438,6 @@
     <t>SADASD</t>
   </si>
   <si>
-    <t>MALE</t>
-  </si>
-  <si>
     <t>white</t>
   </si>
   <si>
@@ -465,17 +459,17 @@
     <t>not provided</t>
   </si>
   <si>
+    <t>CRC0014LM_2</t>
+  </si>
+  <si>
     <t>invalid_sex_value</t>
-  </si>
-  <si>
-    <t>id1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -597,12 +591,6 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -701,7 +689,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -802,9 +790,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1191,7 +1176,7 @@
   <dimension ref="A1:AMJ110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -1254,14 +1239,14 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>85</v>
@@ -1270,17 +1255,10 @@
         <v>11</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A4" s="36" t="s">
-        <v>124</v>
-      </c>
-      <c r="B4" s="36" t="s">
-        <v>123</v>
-      </c>
-    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="5" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="6" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="7" spans="1:7" ht="15.75" customHeight="1"/>
@@ -1397,8 +1375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ977"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView topLeftCell="Q1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -1553,21 +1531,21 @@
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>109</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>110</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>36</v>
@@ -1585,7 +1563,7 @@
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>42</v>
@@ -1593,7 +1571,7 @@
       <c r="R3" s="4"/>
       <c r="S3" s="15"/>
       <c r="T3" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75" customHeight="1"/>
@@ -2580,8 +2558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ979"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -2629,7 +2607,7 @@
     </row>
     <row r="2" spans="1:9" ht="34">
       <c r="A2" s="4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>53</v>
@@ -2658,31 +2636,31 @@
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>52</v>
+        <v>112</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>56</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>102</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1"/>
@@ -3672,7 +3650,7 @@
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -3719,7 +3697,7 @@
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>103</v>
@@ -3745,7 +3723,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3802,7 +3780,7 @@
         <v>84</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H2" s="33" t="s">
         <v>97</v>
@@ -3816,7 +3794,7 @@
     </row>
     <row r="3" spans="1:10" ht="102">
       <c r="A3" s="24" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>83</v>
@@ -3830,7 +3808,7 @@
       <c r="E3" s="26"/>
       <c r="F3" s="26"/>
       <c r="G3" s="34" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H3" s="33" t="s">
         <v>98</v>
@@ -3938,7 +3916,7 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>74</v>

</xml_diff>